<commit_message>
up macro a parte
</commit_message>
<xml_diff>
--- a/Lista_nomes.xlsx
+++ b/Lista_nomes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergio/Documents/WIP/vba/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5514E699-BE41-B34A-9A88-9276904025AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDBF3F46-8BE1-3C4B-9B51-7A6552BAD51A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16400" xr2:uid="{8889B69D-180E-D040-A041-DC3178458682}"/>
+    <workbookView xWindow="1160" yWindow="1600" windowWidth="27640" windowHeight="16400" xr2:uid="{8889B69D-180E-D040-A041-DC3178458682}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>Nome</t>
   </si>
@@ -43,19 +43,7 @@
     <t>idade</t>
   </si>
   <si>
-    <t>paste</t>
-  </si>
-  <si>
-    <t>n1</t>
-  </si>
-  <si>
-    <t>n2</t>
-  </si>
-  <si>
-    <t>n10</t>
-  </si>
-  <si>
-    <t>n4</t>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -87,7 +75,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -423,15 +411,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{767C4E5E-85E3-4F41-AC1B-FEAD8587981D}">
   <sheetPr codeName="Planilha1"/>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -439,36 +427,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>

</xml_diff>